<commit_message>
More one time usign it
</commit_message>
<xml_diff>
--- a/src/main/resources/baseFiles/excel/LastCheckSheet.xlsx
+++ b/src/main/resources/baseFiles/excel/LastCheckSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14440"/>
+    <workbookView windowWidth="24680" windowHeight="14120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -679,11 +679,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1228,7 +1225,7 @@
   <dimension ref="A1:J263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J252"/>
+      <selection activeCell="B2" sqref="A2:J671"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1281,80 +1278,44 @@
       <c r="J2" s="1"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
     </row>
     <row r="22" spans="7:8">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
     </row>
     <row r="48" spans="7:8">
       <c r="G48" s="1"/>
@@ -1377,16 +1338,16 @@
       <c r="J59" s="1"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1"/>
@@ -1401,7 +1362,7 @@
       <c r="J68" s="1"/>
     </row>
     <row r="77" spans="3:8">
-      <c r="C77" s="3"/>
+      <c r="C77" s="2"/>
       <c r="D77"/>
       <c r="E77"/>
       <c r="F77"/>
@@ -1409,40 +1370,40 @@
       <c r="H77" s="1"/>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
     </row>
     <row r="86" spans="7:8">
       <c r="G86" s="1"/>
@@ -1457,116 +1418,116 @@
       <c r="H101" s="1"/>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
     </row>
     <row r="112" spans="1:10">
-      <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
-      <c r="J112" s="2"/>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
     </row>
     <row r="116" spans="1:10">
-      <c r="A116" s="2"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+      <c r="J116" s="1"/>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="2"/>
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
-      <c r="I128" s="2"/>
-      <c r="J128" s="2"/>
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="1"/>
     </row>
     <row r="141" spans="1:10">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
-      <c r="J141" s="2"/>
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
-      <c r="I143" s="2"/>
-      <c r="J143" s="2"/>
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+      <c r="J143" s="1"/>
     </row>
     <row r="145" spans="7:8">
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
     <row r="155" spans="1:10">
-      <c r="A155" s="2"/>
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
-      <c r="G155" s="2"/>
-      <c r="H155" s="2"/>
-      <c r="I155" s="2"/>
-      <c r="J155" s="2"/>
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
     </row>
     <row r="159" spans="1:10">
       <c r="A159" s="1"/>
@@ -1600,18 +1561,6 @@
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
     </row>
-    <row r="212" spans="1:10">
-      <c r="A212" s="1"/>
-      <c r="B212" s="1"/>
-      <c r="C212" s="1"/>
-      <c r="D212" s="1"/>
-      <c r="E212" s="1"/>
-      <c r="F212" s="1"/>
-      <c r="G212" s="1"/>
-      <c r="H212" s="1"/>
-      <c r="I212" s="1"/>
-      <c r="J212" s="1"/>
-    </row>
     <row r="219" spans="1:10">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
@@ -1657,40 +1606,40 @@
       <c r="H242" s="1"/>
     </row>
     <row r="243" spans="1:10">
-      <c r="A243" s="2"/>
-      <c r="B243" s="2"/>
-      <c r="C243" s="2"/>
-      <c r="D243" s="2"/>
-      <c r="E243" s="2"/>
-      <c r="F243" s="2"/>
-      <c r="G243" s="2"/>
-      <c r="H243" s="2"/>
-      <c r="I243" s="2"/>
-      <c r="J243" s="2"/>
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
+      <c r="C243" s="1"/>
+      <c r="D243" s="1"/>
+      <c r="E243" s="1"/>
+      <c r="F243" s="1"/>
+      <c r="G243" s="1"/>
+      <c r="H243" s="1"/>
+      <c r="I243" s="1"/>
+      <c r="J243" s="1"/>
     </row>
     <row r="244" spans="1:10">
-      <c r="A244" s="2"/>
-      <c r="B244" s="2"/>
-      <c r="C244" s="2"/>
-      <c r="D244" s="2"/>
-      <c r="E244" s="2"/>
-      <c r="F244" s="2"/>
-      <c r="G244" s="2"/>
-      <c r="H244" s="2"/>
-      <c r="I244" s="2"/>
-      <c r="J244" s="2"/>
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
+      <c r="D244" s="1"/>
+      <c r="E244" s="1"/>
+      <c r="F244" s="1"/>
+      <c r="G244" s="1"/>
+      <c r="H244" s="1"/>
+      <c r="I244" s="1"/>
+      <c r="J244" s="1"/>
     </row>
     <row r="245" spans="1:10">
-      <c r="A245" s="2"/>
-      <c r="B245" s="2"/>
-      <c r="C245" s="2"/>
-      <c r="D245" s="2"/>
-      <c r="E245" s="2"/>
-      <c r="F245" s="2"/>
-      <c r="G245" s="2"/>
-      <c r="H245" s="2"/>
-      <c r="I245" s="2"/>
-      <c r="J245" s="2"/>
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
+      <c r="D245" s="1"/>
+      <c r="E245" s="1"/>
+      <c r="F245" s="1"/>
+      <c r="G245" s="1"/>
+      <c r="H245" s="1"/>
+      <c r="I245" s="1"/>
+      <c r="J245" s="1"/>
     </row>
     <row r="247" spans="1:10">
       <c r="A247" s="1"/>
@@ -1705,40 +1654,28 @@
       <c r="J247" s="1"/>
     </row>
     <row r="252" spans="1:10">
-      <c r="A252" s="2"/>
-      <c r="B252" s="2"/>
-      <c r="C252" s="2"/>
-      <c r="D252" s="2"/>
-      <c r="E252" s="2"/>
-      <c r="F252" s="2"/>
-      <c r="G252" s="2"/>
-      <c r="H252" s="2"/>
-      <c r="I252" s="2"/>
-      <c r="J252" s="2"/>
-    </row>
-    <row r="262" spans="1:10">
-      <c r="A262" s="2"/>
-      <c r="B262" s="2"/>
-      <c r="C262" s="2"/>
-      <c r="D262" s="2"/>
-      <c r="E262" s="2"/>
-      <c r="F262" s="2"/>
-      <c r="G262" s="2"/>
-      <c r="H262" s="2"/>
-      <c r="I262" s="2"/>
-      <c r="J262" s="2"/>
+      <c r="A252" s="1"/>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="1"/>
+      <c r="E252" s="1"/>
+      <c r="F252" s="1"/>
+      <c r="G252" s="1"/>
+      <c r="H252" s="1"/>
+      <c r="I252" s="1"/>
+      <c r="J252" s="1"/>
     </row>
     <row r="263" spans="1:10">
-      <c r="A263" s="2"/>
-      <c r="B263" s="2"/>
-      <c r="C263" s="2"/>
-      <c r="D263" s="2"/>
-      <c r="E263" s="2"/>
-      <c r="F263" s="2"/>
-      <c r="G263" s="2"/>
-      <c r="H263" s="2"/>
-      <c r="I263" s="2"/>
-      <c r="J263" s="2"/>
+      <c r="A263" s="1"/>
+      <c r="B263" s="1"/>
+      <c r="C263" s="1"/>
+      <c r="D263" s="1"/>
+      <c r="E263" s="1"/>
+      <c r="F263" s="1"/>
+      <c r="G263" s="1"/>
+      <c r="H263" s="1"/>
+      <c r="I263" s="1"/>
+      <c r="J263" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:J263">

</xml_diff>